<commit_message>
Updates and sketch of a full text
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -35,10 +35,10 @@
     <t xml:space="preserve">Cornell FOIA 2016</t>
   </si>
   <si>
+    <t xml:space="preserve">Fedscope-new</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fedscope-old</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fedscope-new</t>
   </si>
   <si>
     <t xml:space="preserve">Common</t>
@@ -371,7 +371,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1537,7 +1537,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>